<commit_message>
Atualizado por script em 03-01-2024 20:45
</commit_message>
<xml_diff>
--- a/2023/iran_persian-gulf-pro-league_2023-2024.xlsx
+++ b/2023/iran_persian-gulf-pro-league_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V116"/>
+  <dimension ref="A1:V117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10693,22 +10693,22 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Aluminium Arak</t>
+          <t>Havadar SC</t>
         </is>
       </c>
       <c r="G112" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Malavan</t>
+          <t>Esteghlal Khuzestan</t>
         </is>
       </c>
       <c r="I112" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J112" t="n">
-        <v>2.52</v>
+        <v>2.24</v>
       </c>
       <c r="K112" t="inlineStr">
         <is>
@@ -10716,15 +10716,15 @@
         </is>
       </c>
       <c r="L112" t="n">
-        <v>2.87</v>
+        <v>2.32</v>
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>31/12/2023 12:13</t>
+          <t>31/12/2023 12:26</t>
         </is>
       </c>
       <c r="N112" t="n">
-        <v>2.58</v>
+        <v>2.69</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -10732,15 +10732,15 @@
         </is>
       </c>
       <c r="P112" t="n">
-        <v>2.34</v>
+        <v>2.61</v>
       </c>
       <c r="Q112" t="inlineStr">
         <is>
-          <t>31/12/2023 12:13</t>
+          <t>31/12/2023 12:26</t>
         </is>
       </c>
       <c r="R112" t="n">
-        <v>3.11</v>
+        <v>3.48</v>
       </c>
       <c r="S112" t="inlineStr">
         <is>
@@ -10748,16 +10748,16 @@
         </is>
       </c>
       <c r="T112" t="n">
-        <v>3.39</v>
+        <v>3.9</v>
       </c>
       <c r="U112" t="inlineStr">
         <is>
-          <t>31/12/2023 12:18</t>
+          <t>31/12/2023 12:26</t>
         </is>
       </c>
       <c r="V112" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/iran/persian-gulf-pro-league/aluminium-arak-malavan/xQBvyFg5/</t>
+          <t>https://www.betexplorer.com/football/iran/persian-gulf-pro-league/havadar-sc-esteghlal-khuzestan/bZCzxeva/</t>
         </is>
       </c>
     </row>
@@ -10785,22 +10785,22 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Havadar SC</t>
+          <t>Aluminium Arak</t>
         </is>
       </c>
       <c r="G113" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Esteghlal Khuzestan</t>
+          <t>Malavan</t>
         </is>
       </c>
       <c r="I113" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J113" t="n">
-        <v>2.24</v>
+        <v>2.52</v>
       </c>
       <c r="K113" t="inlineStr">
         <is>
@@ -10808,15 +10808,15 @@
         </is>
       </c>
       <c r="L113" t="n">
-        <v>2.32</v>
+        <v>2.87</v>
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>31/12/2023 12:26</t>
+          <t>31/12/2023 12:13</t>
         </is>
       </c>
       <c r="N113" t="n">
-        <v>2.69</v>
+        <v>2.58</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -10824,15 +10824,15 @@
         </is>
       </c>
       <c r="P113" t="n">
-        <v>2.61</v>
+        <v>2.34</v>
       </c>
       <c r="Q113" t="inlineStr">
         <is>
-          <t>31/12/2023 12:26</t>
+          <t>31/12/2023 12:13</t>
         </is>
       </c>
       <c r="R113" t="n">
-        <v>3.48</v>
+        <v>3.11</v>
       </c>
       <c r="S113" t="inlineStr">
         <is>
@@ -10840,16 +10840,16 @@
         </is>
       </c>
       <c r="T113" t="n">
-        <v>3.9</v>
+        <v>3.39</v>
       </c>
       <c r="U113" t="inlineStr">
         <is>
-          <t>31/12/2023 12:26</t>
+          <t>31/12/2023 12:18</t>
         </is>
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/iran/persian-gulf-pro-league/havadar-sc-esteghlal-khuzestan/bZCzxeva/</t>
+          <t>https://www.betexplorer.com/football/iran/persian-gulf-pro-league/aluminium-arak-malavan/xQBvyFg5/</t>
         </is>
       </c>
     </row>
@@ -11126,6 +11126,98 @@
       <c r="V116" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/iran/persian-gulf-pro-league/zob-ahan-gol-gohar/IZJnZhOH/</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>iran</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>persian-gulf-pro-league</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E117" s="2" t="n">
+        <v>45294.63541666666</v>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Foolad</t>
+        </is>
+      </c>
+      <c r="G117" t="n">
+        <v>1</v>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Nassaji Mazandaran</t>
+        </is>
+      </c>
+      <c r="I117" t="n">
+        <v>0</v>
+      </c>
+      <c r="J117" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>02/01/2024 09:12</t>
+        </is>
+      </c>
+      <c r="L117" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>03/01/2024 15:14</t>
+        </is>
+      </c>
+      <c r="N117" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>02/01/2024 09:12</t>
+        </is>
+      </c>
+      <c r="P117" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>03/01/2024 15:14</t>
+        </is>
+      </c>
+      <c r="R117" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="S117" t="inlineStr">
+        <is>
+          <t>02/01/2024 09:12</t>
+        </is>
+      </c>
+      <c r="T117" t="n">
+        <v>4.69</v>
+      </c>
+      <c r="U117" t="inlineStr">
+        <is>
+          <t>03/01/2024 15:14</t>
+        </is>
+      </c>
+      <c r="V117" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/iran/persian-gulf-pro-league/foolad-mazandaran/QwQ2uUpi/</t>
         </is>
       </c>
     </row>

</xml_diff>